<commit_message>
Implemented custom log and some other fix
</commit_message>
<xml_diff>
--- a/Naukri_REFramework/Data/Config.xlsx
+++ b/Naukri_REFramework/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269F5A10-0003-4E69-8BA5-00EEA58300EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CDD88E-4D16-4370-8217-D88AD759FEA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -187,6 +187,21 @@
   </si>
   <si>
     <t>https://resdex.naukri.com/v2/search/advSearch</t>
+  </si>
+  <si>
+    <t>\\corp-isc-03\CAI India RPA Recruitment Data</t>
+  </si>
+  <si>
+    <t>Profile_Shared_ServerPath</t>
+  </si>
+  <si>
+    <t>Profile_Shared_OnedrivePath</t>
+  </si>
+  <si>
+    <t>Downloaded profiles to be saved in this CAI Server shared path.</t>
+  </si>
+  <si>
+    <t>Downloaded profiles to be saved in this Onedrive path.  C:\Users\sundarsi\OneDrive\CAI_India_RPA_Recruitment_Data</t>
   </si>
 </sst>
 </file>
@@ -555,13 +570,13 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.08984375" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.54296875" customWidth="1"/>
     <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
@@ -647,8 +662,28 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Implemented Email flow and other changes
</commit_message>
<xml_diff>
--- a/Naukri_REFramework/Data/Config.xlsx
+++ b/Naukri_REFramework/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CDD88E-4D16-4370-8217-D88AD759FEA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0184EF37-F98B-471F-990F-A2F614DAEE7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Naukri_Password</t>
   </si>
   <si>
-    <t>artee.pandita@cai.io</t>
-  </si>
-  <si>
     <t>Cai@1234</t>
   </si>
   <si>
@@ -202,6 +199,15 @@
   </si>
   <si>
     <t>Downloaded profiles to be saved in this Onedrive path.  C:\Users\sundarsi\OneDrive\CAI_India_RPA_Recruitment_Data</t>
+  </si>
+  <si>
+    <t>C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Result</t>
+  </si>
+  <si>
+    <t>IsEmailEnable</t>
+  </si>
+  <si>
+    <t>sivaprakasam.sundaram@cai.io</t>
   </si>
 </sst>
 </file>
@@ -570,7 +576,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -643,15 +649,15 @@
         <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" t="s">
-        <v>52</v>
+      <c r="B6" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -659,32 +665,39 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fine tuned Emails and input validation
</commit_message>
<xml_diff>
--- a/Naukri_REFramework/Data/Config.xlsx
+++ b/Naukri_REFramework/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0184EF37-F98B-471F-990F-A2F614DAEE7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8BCB2D-F3FD-490B-9616-CFC7997E6917}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -174,15 +174,6 @@
     <t>Naukri_URL</t>
   </si>
   <si>
-    <t>Naukri_Username</t>
-  </si>
-  <si>
-    <t>Naukri_Password</t>
-  </si>
-  <si>
-    <t>Cai@1234</t>
-  </si>
-  <si>
     <t>https://resdex.naukri.com/v2/search/advSearch</t>
   </si>
   <si>
@@ -195,19 +186,25 @@
     <t>Profile_Shared_OnedrivePath</t>
   </si>
   <si>
-    <t>Downloaded profiles to be saved in this CAI Server shared path.</t>
-  </si>
-  <si>
     <t>Downloaded profiles to be saved in this Onedrive path.  C:\Users\sundarsi\OneDrive\CAI_India_RPA_Recruitment_Data</t>
   </si>
   <si>
-    <t>C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Result</t>
-  </si>
-  <si>
     <t>IsEmailEnable</t>
   </si>
   <si>
-    <t>sivaprakasam.sundaram@cai.io</t>
+    <t>Downloaded profiles to be saved in this CAI Server shared path.(C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Result)</t>
+  </si>
+  <si>
+    <t>Naukri_Credential</t>
+  </si>
+  <si>
+    <t>Error_EmailTo</t>
+  </si>
+  <si>
+    <t>Status_EmailTo</t>
+  </si>
+  <si>
+    <t>caiindia.rpa@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -573,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -649,56 +646,63 @@
         <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
-        <v>52</v>
+      <c r="C7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>57</v>
+      <c r="B8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1683,15 +1687,14 @@
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{32C7C20A-C4A4-4E99-B791-154A3D46FA18}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{5524AC72-1848-4EC1-9B3D-965015883431}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{1ECE6232-4517-4265-8DE5-B24825AF8BF7}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{1ECE6232-4517-4265-8DE5-B24825AF8BF7}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{20F3E673-A3D9-488F-A689-A70CB2E41BC6}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{95F4A055-A783-40F4-8FDE-F390AF353291}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1699,7 +1702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Calculate Client Security Hash for Assignment level 3
</commit_message>
<xml_diff>
--- a/Naukri_REFramework/Data/Config.xlsx
+++ b/Naukri_REFramework/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8BCB2D-F3FD-490B-9616-CFC7997E6917}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0774B412-92F8-422C-9CBE-E398D4D378B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,7 +653,7 @@
       <c r="A6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C6" t="s">
@@ -664,7 +664,7 @@
       <c r="A7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C7" t="s">
@@ -1692,9 +1692,11 @@
     <hyperlink ref="B5" r:id="rId1" xr:uid="{1ECE6232-4517-4265-8DE5-B24825AF8BF7}"/>
     <hyperlink ref="B10" r:id="rId2" xr:uid="{20F3E673-A3D9-488F-A689-A70CB2E41BC6}"/>
     <hyperlink ref="B11" r:id="rId3" xr:uid="{95F4A055-A783-40F4-8FDE-F390AF353291}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{9F755838-8DAD-4A3B-85E6-9E104D09DF41}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{EC274DB0-6989-400F-A225-C69441ECE8B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated main and clean up the process
</commit_message>
<xml_diff>
--- a/Naukri_REFramework/Data/Config.xlsx
+++ b/Naukri_REFramework/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\source\source\RPA\UiPath\github\Naukri_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0774B412-92F8-422C-9CBE-E398D4D378B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1B28B6-EACB-4971-8253-BF29CA9FBF23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -186,15 +186,9 @@
     <t>Profile_Shared_OnedrivePath</t>
   </si>
   <si>
-    <t>Downloaded profiles to be saved in this Onedrive path.  C:\Users\sundarsi\OneDrive\CAI_India_RPA_Recruitment_Data</t>
-  </si>
-  <si>
     <t>IsEmailEnable</t>
   </si>
   <si>
-    <t>Downloaded profiles to be saved in this CAI Server shared path.(C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Result)</t>
-  </si>
-  <si>
     <t>Naukri_Credential</t>
   </si>
   <si>
@@ -205,6 +199,15 @@
   </si>
   <si>
     <t>caiindia.rpa@gmail.com</t>
+  </si>
+  <si>
+    <t>Downloaded profiles to be saved in this CAI Server shared path.(C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Result)/</t>
+  </si>
+  <si>
+    <t>Downloaded profiles to be saved in this Onedrive path.  C:\Users\sundarsi\OneDrive\CAI_India_RPA_Recruitment_Data: \\corp-isc-03\CAI India RPA Recruitment Data</t>
+  </si>
+  <si>
+    <t>C:</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
         <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -665,15 +668,15 @@
         <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -681,26 +684,26 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1693,10 +1696,9 @@
     <hyperlink ref="B10" r:id="rId2" xr:uid="{20F3E673-A3D9-488F-A689-A70CB2E41BC6}"/>
     <hyperlink ref="B11" r:id="rId3" xr:uid="{95F4A055-A783-40F4-8FDE-F390AF353291}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{9F755838-8DAD-4A3B-85E6-9E104D09DF41}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{EC274DB0-6989-400F-A225-C69441ECE8B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>